<commit_message>
Fixed errors in model edge connections.
</commit_message>
<xml_diff>
--- a/testing/WA Earthquake - Water Treatment Plant 120MLD/input/model.xlsx
+++ b/testing/WA Earthquake - Water Treatment Plant 120MLD/input/model.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u72710\Desktop\sifra\testing\WA Earthquake - Water Treatment Plant 120MLD\input\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16440" tabRatio="788" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14685" tabRatio="788" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="system_meta" sheetId="17" r:id="rId1"/>
@@ -30,7 +35,7 @@
     <definedName name="RESTORATION_TIME_UNIT">OFFSET(VALIDATION_TABLES!$C$2,0,0,COUNTA(VALIDATION_TABLES!$C$2:$C$201),1)</definedName>
     <definedName name="SYSTEM_CLASSES">OFFSET(VALIDATION_TABLES!$B$2,0,0,COUNTA(VALIDATION_TABLES!$B$2:$B$201),1)</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1260,7 +1265,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -4447,7 +4452,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5774,7 +5779,7 @@
   </sheetPr>
   <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
     </sheetView>
@@ -7971,7 +7976,7 @@
   </sheetPr>
   <dimension ref="A1:E176"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
     </sheetView>

</xml_diff>